<commit_message>
change info of paper No.447
</commit_message>
<xml_diff>
--- a/content/program/TRISTAN2025_final_program.xlsx
+++ b/content/program/TRISTAN2025_final_program.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masudasatoki/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masudasatoki/Desktop/tristan2025-website/content/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC8CD36-5E32-534A-9B73-2D30DFE4BD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750A71FB-AB7A-F943-B92A-089097A0FFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" activeTab="1" xr2:uid="{6B18BE26-13C5-0449-A7C1-25BFDB85670B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{6B18BE26-13C5-0449-A7C1-25BFDB85670B}"/>
   </bookViews>
   <sheets>
     <sheet name="Program list (2)" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7501" uniqueCount="1095">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7501" uniqueCount="1096">
   <si>
     <t>Humanitarian Logistics</t>
   </si>
@@ -3436,6 +3436,10 @@
   </si>
   <si>
     <t>未決済</t>
+  </si>
+  <si>
+    <t>Minghao Chen, Zhiyuan Shi, Ang Li and Max Z. Li</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -3775,15 +3779,6 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3800,6 +3795,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4144,8 +4148,8 @@
   </sheetPr>
   <dimension ref="A1:G165"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="59" zoomScaleSheetLayoutView="40" zoomScalePageLayoutView="36" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="81" zoomScaleNormal="59" zoomScaleSheetLayoutView="40" zoomScalePageLayoutView="36" workbookViewId="0">
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5703125" defaultRowHeight="31"/>
@@ -4184,16 +4188,16 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="54" t="s">
         <v>1062</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="55" t="s">
         <v>1067</v>
       </c>
-      <c r="C2" s="52">
+      <c r="C2" s="60">
         <v>1</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="54" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="36">
@@ -4207,10 +4211,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="62" customHeight="1">
-      <c r="A3" s="55"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="55"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="52"/>
       <c r="E3" s="29">
         <v>55</v>
       </c>
@@ -4222,10 +4226,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="62" customHeight="1">
-      <c r="A4" s="55"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="55"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="29">
         <v>412</v>
       </c>
@@ -4237,12 +4241,12 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="62" customHeight="1">
-      <c r="A5" s="55"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="53">
+      <c r="A5" s="52"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="58">
         <v>2</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="52" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="29">
@@ -4256,10 +4260,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="62" customHeight="1">
-      <c r="A6" s="55"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="55"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="29">
         <v>253</v>
       </c>
@@ -4271,10 +4275,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="62" customHeight="1">
-      <c r="A7" s="55"/>
-      <c r="B7" s="59"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="55"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="52"/>
       <c r="E7" s="29">
         <v>72</v>
       </c>
@@ -4286,12 +4290,12 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="62" customHeight="1">
-      <c r="A8" s="55"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="53">
+      <c r="A8" s="52"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="58">
         <v>3</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="52" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="29">
@@ -4305,10 +4309,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="62" customHeight="1">
-      <c r="A9" s="55"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="55"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="52"/>
       <c r="E9" s="29">
         <v>37</v>
       </c>
@@ -4320,10 +4324,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A10" s="56"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="56"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="37">
         <v>452</v>
       </c>
@@ -4335,16 +4339,16 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="54" t="s">
         <v>1062</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="55" t="s">
         <v>1068</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="60">
         <v>1</v>
       </c>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="54" t="s">
         <v>191</v>
       </c>
       <c r="E11" s="36">
@@ -4358,10 +4362,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="62" customHeight="1">
-      <c r="A12" s="55"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="55"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="52"/>
       <c r="E12" s="29">
         <v>441</v>
       </c>
@@ -4373,10 +4377,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="62" customHeight="1">
-      <c r="A13" s="55"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="55"/>
+      <c r="A13" s="52"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="52"/>
       <c r="E13" s="29">
         <v>212</v>
       </c>
@@ -4388,12 +4392,12 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="62" customHeight="1">
-      <c r="A14" s="55"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="53">
+      <c r="A14" s="52"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="58">
         <v>2</v>
       </c>
-      <c r="D14" s="55" t="s">
+      <c r="D14" s="52" t="s">
         <v>199</v>
       </c>
       <c r="E14" s="29">
@@ -4407,10 +4411,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="62" customHeight="1">
-      <c r="A15" s="55"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="55"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="52"/>
       <c r="E15" s="29">
         <v>296</v>
       </c>
@@ -4422,10 +4426,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="62" customHeight="1">
-      <c r="A16" s="55"/>
-      <c r="B16" s="59"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="55"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="29">
         <v>457</v>
       </c>
@@ -4437,12 +4441,12 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="62" customHeight="1">
-      <c r="A17" s="55"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="53">
+      <c r="A17" s="52"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="58">
         <v>3</v>
       </c>
-      <c r="D17" s="55" t="s">
+      <c r="D17" s="52" t="s">
         <v>265</v>
       </c>
       <c r="E17" s="29">
@@ -4456,10 +4460,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="62" customHeight="1">
-      <c r="A18" s="55"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="55"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="52"/>
       <c r="E18" s="29">
         <v>211</v>
       </c>
@@ -4471,10 +4475,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A19" s="56"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="56"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="37">
         <v>199</v>
       </c>
@@ -4486,16 +4490,16 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="54" t="s">
         <v>1062</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="55" t="s">
         <v>1069</v>
       </c>
-      <c r="C20" s="52">
+      <c r="C20" s="60">
         <v>1</v>
       </c>
-      <c r="D20" s="57" t="s">
+      <c r="D20" s="54" t="s">
         <v>155</v>
       </c>
       <c r="E20" s="36">
@@ -4509,10 +4513,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="62" customHeight="1">
-      <c r="A21" s="55"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="55"/>
+      <c r="A21" s="52"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="52"/>
       <c r="E21" s="29">
         <v>13</v>
       </c>
@@ -4524,10 +4528,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="62" customHeight="1">
-      <c r="A22" s="55"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="55"/>
+      <c r="A22" s="52"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="52"/>
       <c r="E22" s="29">
         <v>17</v>
       </c>
@@ -4539,10 +4543,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="62" customHeight="1">
-      <c r="A23" s="55"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="55"/>
+      <c r="A23" s="52"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="52"/>
       <c r="E23" s="29">
         <v>148</v>
       </c>
@@ -4554,12 +4558,12 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="62" customHeight="1">
-      <c r="A24" s="55"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="53">
+      <c r="A24" s="52"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="58">
         <v>2</v>
       </c>
-      <c r="D24" s="55" t="s">
+      <c r="D24" s="52" t="s">
         <v>219</v>
       </c>
       <c r="E24" s="29">
@@ -4573,10 +4577,10 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="62" customHeight="1">
-      <c r="A25" s="55"/>
-      <c r="B25" s="59"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="55"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="52"/>
       <c r="E25" s="29">
         <v>247</v>
       </c>
@@ -4588,10 +4592,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="62" customHeight="1">
-      <c r="A26" s="55"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="55"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="52"/>
       <c r="E26" s="29">
         <v>254</v>
       </c>
@@ -4603,10 +4607,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="62" customHeight="1">
-      <c r="A27" s="55"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="55"/>
+      <c r="A27" s="52"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="52"/>
       <c r="E27" s="29">
         <v>143</v>
       </c>
@@ -4618,12 +4622,12 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="62" customHeight="1">
-      <c r="A28" s="55"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="53">
+      <c r="A28" s="52"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="58">
         <v>3</v>
       </c>
-      <c r="D28" s="55" t="s">
+      <c r="D28" s="52" t="s">
         <v>266</v>
       </c>
       <c r="E28" s="29">
@@ -4637,10 +4641,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="62" customHeight="1">
-      <c r="A29" s="55"/>
-      <c r="B29" s="59"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="55"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="52"/>
       <c r="E29" s="29">
         <v>29</v>
       </c>
@@ -4652,10 +4656,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="62" customHeight="1">
-      <c r="A30" s="55"/>
-      <c r="B30" s="59"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="55"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="52"/>
       <c r="E30" s="29">
         <v>404</v>
       </c>
@@ -4667,10 +4671,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A31" s="56"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="56"/>
+      <c r="A31" s="53"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="53"/>
       <c r="E31" s="37">
         <v>15</v>
       </c>
@@ -4682,16 +4686,16 @@
       </c>
     </row>
     <row r="32" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A32" s="57" t="s">
+      <c r="A32" s="54" t="s">
         <v>1062</v>
       </c>
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="55" t="s">
         <v>1070</v>
       </c>
-      <c r="C32" s="52">
+      <c r="C32" s="60">
         <v>1</v>
       </c>
-      <c r="D32" s="57" t="s">
+      <c r="D32" s="54" t="s">
         <v>267</v>
       </c>
       <c r="E32" s="36">
@@ -4705,10 +4709,10 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="62" customHeight="1">
-      <c r="A33" s="55"/>
-      <c r="B33" s="59"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="55"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="52"/>
       <c r="E33" s="29">
         <v>484</v>
       </c>
@@ -4720,10 +4724,10 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="62" customHeight="1">
-      <c r="A34" s="55"/>
-      <c r="B34" s="59"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="55"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="52"/>
       <c r="E34" s="29">
         <v>110</v>
       </c>
@@ -4735,10 +4739,10 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="62" customHeight="1">
-      <c r="A35" s="55"/>
-      <c r="B35" s="59"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="55"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="52"/>
       <c r="E35" s="29">
         <v>144</v>
       </c>
@@ -4750,12 +4754,12 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="62" customHeight="1">
-      <c r="A36" s="55"/>
-      <c r="B36" s="59"/>
-      <c r="C36" s="53">
+      <c r="A36" s="52"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="58">
         <v>2</v>
       </c>
-      <c r="D36" s="55" t="s">
+      <c r="D36" s="52" t="s">
         <v>233</v>
       </c>
       <c r="E36" s="29">
@@ -4769,10 +4773,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="62" customHeight="1">
-      <c r="A37" s="55"/>
-      <c r="B37" s="59"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="55"/>
+      <c r="A37" s="52"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="52"/>
       <c r="E37" s="29">
         <v>385</v>
       </c>
@@ -4784,10 +4788,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="62" customHeight="1">
-      <c r="A38" s="55"/>
-      <c r="B38" s="59"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="55"/>
+      <c r="A38" s="52"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="52"/>
       <c r="E38" s="29">
         <v>160</v>
       </c>
@@ -4799,10 +4803,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="62" customHeight="1">
-      <c r="A39" s="55"/>
-      <c r="B39" s="59"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="55"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="52"/>
       <c r="E39" s="29">
         <v>292</v>
       </c>
@@ -4814,12 +4818,12 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="62" customHeight="1">
-      <c r="A40" s="55"/>
-      <c r="B40" s="59"/>
-      <c r="C40" s="53">
+      <c r="A40" s="52"/>
+      <c r="B40" s="56"/>
+      <c r="C40" s="58">
         <v>3</v>
       </c>
-      <c r="D40" s="55" t="s">
+      <c r="D40" s="52" t="s">
         <v>186</v>
       </c>
       <c r="E40" s="29">
@@ -4833,10 +4837,10 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="62" customHeight="1">
-      <c r="A41" s="55"/>
-      <c r="B41" s="59"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="55"/>
+      <c r="A41" s="52"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="52"/>
       <c r="E41" s="29">
         <v>278</v>
       </c>
@@ -4848,10 +4852,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="62" customHeight="1">
-      <c r="A42" s="55"/>
-      <c r="B42" s="59"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="55"/>
+      <c r="A42" s="52"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="52"/>
       <c r="E42" s="29">
         <v>181</v>
       </c>
@@ -4863,10 +4867,10 @@
       </c>
     </row>
     <row r="43" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A43" s="56"/>
-      <c r="B43" s="60"/>
-      <c r="C43" s="54"/>
-      <c r="D43" s="56"/>
+      <c r="A43" s="53"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="53"/>
       <c r="E43" s="37">
         <v>464</v>
       </c>
@@ -4878,16 +4882,16 @@
       </c>
     </row>
     <row r="44" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A44" s="57" t="s">
+      <c r="A44" s="54" t="s">
         <v>1063</v>
       </c>
-      <c r="B44" s="58" t="s">
+      <c r="B44" s="55" t="s">
         <v>1067</v>
       </c>
-      <c r="C44" s="52">
+      <c r="C44" s="60">
         <v>1</v>
       </c>
-      <c r="D44" s="57" t="s">
+      <c r="D44" s="54" t="s">
         <v>268</v>
       </c>
       <c r="E44" s="36">
@@ -4901,10 +4905,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="62" customHeight="1">
-      <c r="A45" s="55"/>
-      <c r="B45" s="59"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="55"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="52"/>
       <c r="E45" s="29">
         <v>204</v>
       </c>
@@ -4916,10 +4920,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="62" customHeight="1">
-      <c r="A46" s="55"/>
-      <c r="B46" s="59"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="55"/>
+      <c r="A46" s="52"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="52"/>
       <c r="E46" s="29">
         <v>206</v>
       </c>
@@ -4931,12 +4935,12 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="62" customHeight="1">
-      <c r="A47" s="55"/>
-      <c r="B47" s="59"/>
-      <c r="C47" s="53">
+      <c r="A47" s="52"/>
+      <c r="B47" s="56"/>
+      <c r="C47" s="58">
         <v>2</v>
       </c>
-      <c r="D47" s="55" t="s">
+      <c r="D47" s="52" t="s">
         <v>269</v>
       </c>
       <c r="E47" s="29">
@@ -4950,10 +4954,10 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="62" customHeight="1">
-      <c r="A48" s="55"/>
-      <c r="B48" s="59"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="55"/>
+      <c r="A48" s="52"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="52"/>
       <c r="E48" s="29">
         <v>213</v>
       </c>
@@ -4965,10 +4969,10 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="62" customHeight="1">
-      <c r="A49" s="55"/>
-      <c r="B49" s="59"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="55"/>
+      <c r="A49" s="52"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="52"/>
       <c r="E49" s="29">
         <v>141</v>
       </c>
@@ -4980,12 +4984,12 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="62" customHeight="1">
-      <c r="A50" s="55"/>
-      <c r="B50" s="59"/>
-      <c r="C50" s="53">
+      <c r="A50" s="52"/>
+      <c r="B50" s="56"/>
+      <c r="C50" s="58">
         <v>3</v>
       </c>
-      <c r="D50" s="55" t="s">
+      <c r="D50" s="52" t="s">
         <v>261</v>
       </c>
       <c r="E50" s="29">
@@ -4999,10 +5003,10 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="62" customHeight="1">
-      <c r="A51" s="55"/>
-      <c r="B51" s="59"/>
-      <c r="C51" s="53"/>
-      <c r="D51" s="55"/>
+      <c r="A51" s="52"/>
+      <c r="B51" s="56"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="52"/>
       <c r="E51" s="29">
         <v>91</v>
       </c>
@@ -5014,10 +5018,10 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="62" customHeight="1" thickBot="1">
-      <c r="A52" s="56"/>
-      <c r="B52" s="60"/>
-      <c r="C52" s="54"/>
-      <c r="D52" s="56"/>
+      <c r="A52" s="53"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="53"/>
       <c r="E52" s="29">
         <v>65</v>
       </c>
@@ -5029,16 +5033,16 @@
       </c>
     </row>
     <row r="53" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A53" s="57" t="s">
+      <c r="A53" s="54" t="s">
         <v>1063</v>
       </c>
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="55" t="s">
         <v>1068</v>
       </c>
-      <c r="C53" s="52">
+      <c r="C53" s="60">
         <v>1</v>
       </c>
-      <c r="D53" s="57" t="s">
+      <c r="D53" s="54" t="s">
         <v>270</v>
       </c>
       <c r="E53" s="36">
@@ -5052,10 +5056,10 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="62" customHeight="1">
-      <c r="A54" s="55"/>
-      <c r="B54" s="59"/>
-      <c r="C54" s="53"/>
-      <c r="D54" s="55"/>
+      <c r="A54" s="52"/>
+      <c r="B54" s="56"/>
+      <c r="C54" s="58"/>
+      <c r="D54" s="52"/>
       <c r="E54" s="29">
         <v>433</v>
       </c>
@@ -5067,10 +5071,10 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="62" customHeight="1">
-      <c r="A55" s="55"/>
-      <c r="B55" s="59"/>
-      <c r="C55" s="53"/>
-      <c r="D55" s="55"/>
+      <c r="A55" s="52"/>
+      <c r="B55" s="56"/>
+      <c r="C55" s="58"/>
+      <c r="D55" s="52"/>
       <c r="E55" s="29">
         <v>163</v>
       </c>
@@ -5082,12 +5086,12 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="62" customHeight="1">
-      <c r="A56" s="55"/>
-      <c r="B56" s="59"/>
-      <c r="C56" s="53">
+      <c r="A56" s="52"/>
+      <c r="B56" s="56"/>
+      <c r="C56" s="58">
         <v>2</v>
       </c>
-      <c r="D56" s="55" t="s">
+      <c r="D56" s="52" t="s">
         <v>271</v>
       </c>
       <c r="E56" s="29">
@@ -5101,10 +5105,10 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="62" customHeight="1">
-      <c r="A57" s="55"/>
-      <c r="B57" s="59"/>
-      <c r="C57" s="53"/>
-      <c r="D57" s="55"/>
+      <c r="A57" s="52"/>
+      <c r="B57" s="56"/>
+      <c r="C57" s="58"/>
+      <c r="D57" s="52"/>
       <c r="E57" s="29">
         <v>257</v>
       </c>
@@ -5116,10 +5120,10 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="62" customHeight="1">
-      <c r="A58" s="55"/>
-      <c r="B58" s="59"/>
-      <c r="C58" s="53"/>
-      <c r="D58" s="55"/>
+      <c r="A58" s="52"/>
+      <c r="B58" s="56"/>
+      <c r="C58" s="58"/>
+      <c r="D58" s="52"/>
       <c r="E58" s="29">
         <v>344</v>
       </c>
@@ -5131,12 +5135,12 @@
       </c>
     </row>
     <row r="59" spans="1:7" ht="62" customHeight="1">
-      <c r="A59" s="55"/>
-      <c r="B59" s="59"/>
-      <c r="C59" s="53">
+      <c r="A59" s="52"/>
+      <c r="B59" s="56"/>
+      <c r="C59" s="58">
         <v>3</v>
       </c>
-      <c r="D59" s="55" t="s">
+      <c r="D59" s="52" t="s">
         <v>238</v>
       </c>
       <c r="E59" s="29">
@@ -5150,10 +5154,10 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="62" customHeight="1">
-      <c r="A60" s="55"/>
-      <c r="B60" s="59"/>
-      <c r="C60" s="53"/>
-      <c r="D60" s="55"/>
+      <c r="A60" s="52"/>
+      <c r="B60" s="56"/>
+      <c r="C60" s="58"/>
+      <c r="D60" s="52"/>
       <c r="E60" s="29">
         <v>276</v>
       </c>
@@ -5165,10 +5169,10 @@
       </c>
     </row>
     <row r="61" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A61" s="56"/>
-      <c r="B61" s="60"/>
-      <c r="C61" s="54"/>
-      <c r="D61" s="56"/>
+      <c r="A61" s="53"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="53"/>
       <c r="E61" s="37">
         <v>366</v>
       </c>
@@ -5180,16 +5184,16 @@
       </c>
     </row>
     <row r="62" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A62" s="57" t="s">
+      <c r="A62" s="54" t="s">
         <v>1063</v>
       </c>
-      <c r="B62" s="58" t="s">
+      <c r="B62" s="55" t="s">
         <v>1069</v>
       </c>
-      <c r="C62" s="52">
+      <c r="C62" s="60">
         <v>1</v>
       </c>
-      <c r="D62" s="57" t="s">
+      <c r="D62" s="54" t="s">
         <v>272</v>
       </c>
       <c r="E62" s="36">
@@ -5203,10 +5207,10 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="62" customHeight="1">
-      <c r="A63" s="55"/>
-      <c r="B63" s="59"/>
-      <c r="C63" s="53"/>
-      <c r="D63" s="55"/>
+      <c r="A63" s="52"/>
+      <c r="B63" s="56"/>
+      <c r="C63" s="58"/>
+      <c r="D63" s="52"/>
       <c r="E63" s="29">
         <v>351</v>
       </c>
@@ -5218,10 +5222,10 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="62" customHeight="1">
-      <c r="A64" s="55"/>
-      <c r="B64" s="59"/>
-      <c r="C64" s="53"/>
-      <c r="D64" s="55"/>
+      <c r="A64" s="52"/>
+      <c r="B64" s="56"/>
+      <c r="C64" s="58"/>
+      <c r="D64" s="52"/>
       <c r="E64" s="29">
         <v>489</v>
       </c>
@@ -5233,10 +5237,10 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="62" customHeight="1">
-      <c r="A65" s="55"/>
-      <c r="B65" s="59"/>
-      <c r="C65" s="53"/>
-      <c r="D65" s="55"/>
+      <c r="A65" s="52"/>
+      <c r="B65" s="56"/>
+      <c r="C65" s="58"/>
+      <c r="D65" s="52"/>
       <c r="E65" s="29">
         <v>16</v>
       </c>
@@ -5248,12 +5252,12 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="62" customHeight="1">
-      <c r="A66" s="55"/>
-      <c r="B66" s="59"/>
-      <c r="C66" s="53">
+      <c r="A66" s="52"/>
+      <c r="B66" s="56"/>
+      <c r="C66" s="58">
         <v>2</v>
       </c>
-      <c r="D66" s="55" t="s">
+      <c r="D66" s="52" t="s">
         <v>228</v>
       </c>
       <c r="E66" s="29">
@@ -5267,10 +5271,10 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="62" customHeight="1">
-      <c r="A67" s="55"/>
-      <c r="B67" s="59"/>
-      <c r="C67" s="53"/>
-      <c r="D67" s="55"/>
+      <c r="A67" s="52"/>
+      <c r="B67" s="56"/>
+      <c r="C67" s="58"/>
+      <c r="D67" s="52"/>
       <c r="E67" s="29">
         <v>58</v>
       </c>
@@ -5282,10 +5286,10 @@
       </c>
     </row>
     <row r="68" spans="1:7" ht="62" customHeight="1">
-      <c r="A68" s="55"/>
-      <c r="B68" s="59"/>
-      <c r="C68" s="53"/>
-      <c r="D68" s="55"/>
+      <c r="A68" s="52"/>
+      <c r="B68" s="56"/>
+      <c r="C68" s="58"/>
+      <c r="D68" s="52"/>
       <c r="E68" s="29">
         <v>115</v>
       </c>
@@ -5297,10 +5301,10 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="62" customHeight="1">
-      <c r="A69" s="55"/>
-      <c r="B69" s="59"/>
-      <c r="C69" s="53"/>
-      <c r="D69" s="55"/>
+      <c r="A69" s="52"/>
+      <c r="B69" s="56"/>
+      <c r="C69" s="58"/>
+      <c r="D69" s="52"/>
       <c r="E69" s="29">
         <v>130</v>
       </c>
@@ -5312,12 +5316,12 @@
       </c>
     </row>
     <row r="70" spans="1:7" ht="62" customHeight="1">
-      <c r="A70" s="55"/>
-      <c r="B70" s="59"/>
-      <c r="C70" s="53">
+      <c r="A70" s="52"/>
+      <c r="B70" s="56"/>
+      <c r="C70" s="58">
         <v>3</v>
       </c>
-      <c r="D70" s="55" t="s">
+      <c r="D70" s="52" t="s">
         <v>43</v>
       </c>
       <c r="E70" s="29">
@@ -5331,10 +5335,10 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="62" customHeight="1">
-      <c r="A71" s="55"/>
-      <c r="B71" s="59"/>
-      <c r="C71" s="53"/>
-      <c r="D71" s="55"/>
+      <c r="A71" s="52"/>
+      <c r="B71" s="56"/>
+      <c r="C71" s="58"/>
+      <c r="D71" s="52"/>
       <c r="E71" s="29">
         <v>329</v>
       </c>
@@ -5346,10 +5350,10 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="62" customHeight="1">
-      <c r="A72" s="55"/>
-      <c r="B72" s="59"/>
-      <c r="C72" s="53"/>
-      <c r="D72" s="55"/>
+      <c r="A72" s="52"/>
+      <c r="B72" s="56"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="52"/>
       <c r="E72" s="29">
         <v>474</v>
       </c>
@@ -5361,10 +5365,10 @@
       </c>
     </row>
     <row r="73" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A73" s="56"/>
-      <c r="B73" s="60"/>
-      <c r="C73" s="54"/>
-      <c r="D73" s="56"/>
+      <c r="A73" s="53"/>
+      <c r="B73" s="57"/>
+      <c r="C73" s="59"/>
+      <c r="D73" s="53"/>
       <c r="E73" s="37">
         <v>283</v>
       </c>
@@ -5376,16 +5380,16 @@
       </c>
     </row>
     <row r="74" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A74" s="57" t="s">
+      <c r="A74" s="54" t="s">
         <v>1063</v>
       </c>
-      <c r="B74" s="58" t="s">
+      <c r="B74" s="55" t="s">
         <v>1070</v>
       </c>
-      <c r="C74" s="52">
+      <c r="C74" s="60">
         <v>1</v>
       </c>
-      <c r="D74" s="57" t="s">
+      <c r="D74" s="54" t="s">
         <v>273</v>
       </c>
       <c r="E74" s="36">
@@ -5399,10 +5403,10 @@
       </c>
     </row>
     <row r="75" spans="1:7" ht="62" customHeight="1">
-      <c r="A75" s="55"/>
-      <c r="B75" s="59"/>
-      <c r="C75" s="53"/>
-      <c r="D75" s="55"/>
+      <c r="A75" s="52"/>
+      <c r="B75" s="56"/>
+      <c r="C75" s="58"/>
+      <c r="D75" s="52"/>
       <c r="E75" s="29">
         <v>275</v>
       </c>
@@ -5414,10 +5418,10 @@
       </c>
     </row>
     <row r="76" spans="1:7" ht="62" customHeight="1">
-      <c r="A76" s="55"/>
-      <c r="B76" s="59"/>
-      <c r="C76" s="53"/>
-      <c r="D76" s="55"/>
+      <c r="A76" s="52"/>
+      <c r="B76" s="56"/>
+      <c r="C76" s="58"/>
+      <c r="D76" s="52"/>
       <c r="E76" s="29">
         <v>348</v>
       </c>
@@ -5429,10 +5433,10 @@
       </c>
     </row>
     <row r="77" spans="1:7" ht="62" customHeight="1">
-      <c r="A77" s="55"/>
-      <c r="B77" s="59"/>
-      <c r="C77" s="53"/>
-      <c r="D77" s="55"/>
+      <c r="A77" s="52"/>
+      <c r="B77" s="56"/>
+      <c r="C77" s="58"/>
+      <c r="D77" s="52"/>
       <c r="E77" s="29">
         <v>191</v>
       </c>
@@ -5444,12 +5448,12 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="62" customHeight="1">
-      <c r="A78" s="55"/>
-      <c r="B78" s="59"/>
-      <c r="C78" s="53">
+      <c r="A78" s="52"/>
+      <c r="B78" s="56"/>
+      <c r="C78" s="58">
         <v>2</v>
       </c>
-      <c r="D78" s="55" t="s">
+      <c r="D78" s="52" t="s">
         <v>274</v>
       </c>
       <c r="E78" s="29">
@@ -5463,10 +5467,10 @@
       </c>
     </row>
     <row r="79" spans="1:7" ht="62" customHeight="1">
-      <c r="A79" s="55"/>
-      <c r="B79" s="59"/>
-      <c r="C79" s="53"/>
-      <c r="D79" s="55"/>
+      <c r="A79" s="52"/>
+      <c r="B79" s="56"/>
+      <c r="C79" s="58"/>
+      <c r="D79" s="52"/>
       <c r="E79" s="29">
         <v>419</v>
       </c>
@@ -5478,10 +5482,10 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="62" customHeight="1">
-      <c r="A80" s="55"/>
-      <c r="B80" s="59"/>
-      <c r="C80" s="53"/>
-      <c r="D80" s="55"/>
+      <c r="A80" s="52"/>
+      <c r="B80" s="56"/>
+      <c r="C80" s="58"/>
+      <c r="D80" s="52"/>
       <c r="E80" s="29">
         <v>357</v>
       </c>
@@ -5493,10 +5497,10 @@
       </c>
     </row>
     <row r="81" spans="1:7" ht="62" customHeight="1">
-      <c r="A81" s="55"/>
-      <c r="B81" s="59"/>
-      <c r="C81" s="53"/>
-      <c r="D81" s="55"/>
+      <c r="A81" s="52"/>
+      <c r="B81" s="56"/>
+      <c r="C81" s="58"/>
+      <c r="D81" s="52"/>
       <c r="E81" s="29">
         <v>19</v>
       </c>
@@ -5508,12 +5512,12 @@
       </c>
     </row>
     <row r="82" spans="1:7" ht="62" customHeight="1">
-      <c r="A82" s="55"/>
-      <c r="B82" s="59"/>
-      <c r="C82" s="53">
+      <c r="A82" s="52"/>
+      <c r="B82" s="56"/>
+      <c r="C82" s="58">
         <v>3</v>
       </c>
-      <c r="D82" s="55" t="s">
+      <c r="D82" s="52" t="s">
         <v>275</v>
       </c>
       <c r="E82" s="29">
@@ -5527,10 +5531,10 @@
       </c>
     </row>
     <row r="83" spans="1:7" ht="62" customHeight="1">
-      <c r="A83" s="55"/>
-      <c r="B83" s="59"/>
-      <c r="C83" s="53"/>
-      <c r="D83" s="55"/>
+      <c r="A83" s="52"/>
+      <c r="B83" s="56"/>
+      <c r="C83" s="58"/>
+      <c r="D83" s="52"/>
       <c r="E83" s="29">
         <v>5</v>
       </c>
@@ -5542,10 +5546,10 @@
       </c>
     </row>
     <row r="84" spans="1:7" ht="62" customHeight="1">
-      <c r="A84" s="55"/>
-      <c r="B84" s="59"/>
-      <c r="C84" s="53"/>
-      <c r="D84" s="55"/>
+      <c r="A84" s="52"/>
+      <c r="B84" s="56"/>
+      <c r="C84" s="58"/>
+      <c r="D84" s="52"/>
       <c r="E84" s="29">
         <v>268</v>
       </c>
@@ -5557,10 +5561,10 @@
       </c>
     </row>
     <row r="85" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A85" s="56"/>
-      <c r="B85" s="60"/>
-      <c r="C85" s="54"/>
-      <c r="D85" s="56"/>
+      <c r="A85" s="53"/>
+      <c r="B85" s="57"/>
+      <c r="C85" s="59"/>
+      <c r="D85" s="53"/>
       <c r="E85" s="37">
         <v>325</v>
       </c>
@@ -5572,16 +5576,16 @@
       </c>
     </row>
     <row r="86" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A86" s="57" t="s">
+      <c r="A86" s="54" t="s">
         <v>1064</v>
       </c>
-      <c r="B86" s="58" t="s">
+      <c r="B86" s="55" t="s">
         <v>1067</v>
       </c>
-      <c r="C86" s="52">
+      <c r="C86" s="60">
         <v>1</v>
       </c>
-      <c r="D86" s="57" t="s">
+      <c r="D86" s="54" t="s">
         <v>579</v>
       </c>
       <c r="E86" s="36">
@@ -5595,10 +5599,10 @@
       </c>
     </row>
     <row r="87" spans="1:7" ht="62" customHeight="1">
-      <c r="A87" s="55"/>
-      <c r="B87" s="59"/>
-      <c r="C87" s="53"/>
-      <c r="D87" s="55"/>
+      <c r="A87" s="52"/>
+      <c r="B87" s="56"/>
+      <c r="C87" s="58"/>
+      <c r="D87" s="52"/>
       <c r="E87" s="29">
         <v>150</v>
       </c>
@@ -5610,10 +5614,10 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="62" customHeight="1">
-      <c r="A88" s="55"/>
-      <c r="B88" s="59"/>
-      <c r="C88" s="53"/>
-      <c r="D88" s="55"/>
+      <c r="A88" s="52"/>
+      <c r="B88" s="56"/>
+      <c r="C88" s="58"/>
+      <c r="D88" s="52"/>
       <c r="E88" s="29">
         <v>117</v>
       </c>
@@ -5625,12 +5629,12 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="62" customHeight="1">
-      <c r="A89" s="55"/>
-      <c r="B89" s="59"/>
-      <c r="C89" s="53">
+      <c r="A89" s="52"/>
+      <c r="B89" s="56"/>
+      <c r="C89" s="58">
         <v>2</v>
       </c>
-      <c r="D89" s="55" t="s">
+      <c r="D89" s="52" t="s">
         <v>51</v>
       </c>
       <c r="E89" s="29">
@@ -5644,10 +5648,10 @@
       </c>
     </row>
     <row r="90" spans="1:7" ht="62" customHeight="1">
-      <c r="A90" s="55"/>
-      <c r="B90" s="59"/>
-      <c r="C90" s="53"/>
-      <c r="D90" s="55"/>
+      <c r="A90" s="52"/>
+      <c r="B90" s="56"/>
+      <c r="C90" s="58"/>
+      <c r="D90" s="52"/>
       <c r="E90" s="29">
         <v>133</v>
       </c>
@@ -5659,10 +5663,10 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="62" customHeight="1">
-      <c r="A91" s="55"/>
-      <c r="B91" s="59"/>
-      <c r="C91" s="53"/>
-      <c r="D91" s="55"/>
+      <c r="A91" s="52"/>
+      <c r="B91" s="56"/>
+      <c r="C91" s="58"/>
+      <c r="D91" s="52"/>
       <c r="E91" s="29">
         <v>242</v>
       </c>
@@ -5674,12 +5678,12 @@
       </c>
     </row>
     <row r="92" spans="1:7" ht="62" customHeight="1">
-      <c r="A92" s="55"/>
-      <c r="B92" s="59"/>
-      <c r="C92" s="53">
+      <c r="A92" s="52"/>
+      <c r="B92" s="56"/>
+      <c r="C92" s="58">
         <v>3</v>
       </c>
-      <c r="D92" s="55" t="s">
+      <c r="D92" s="52" t="s">
         <v>242</v>
       </c>
       <c r="E92" s="29">
@@ -5693,10 +5697,10 @@
       </c>
     </row>
     <row r="93" spans="1:7" ht="62" customHeight="1">
-      <c r="A93" s="55"/>
-      <c r="B93" s="59"/>
-      <c r="C93" s="53"/>
-      <c r="D93" s="55"/>
+      <c r="A93" s="52"/>
+      <c r="B93" s="56"/>
+      <c r="C93" s="58"/>
+      <c r="D93" s="52"/>
       <c r="E93" s="29">
         <v>304</v>
       </c>
@@ -5708,10 +5712,10 @@
       </c>
     </row>
     <row r="94" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A94" s="56"/>
-      <c r="B94" s="60"/>
-      <c r="C94" s="54"/>
-      <c r="D94" s="56"/>
+      <c r="A94" s="53"/>
+      <c r="B94" s="57"/>
+      <c r="C94" s="59"/>
+      <c r="D94" s="53"/>
       <c r="E94" s="37">
         <v>316</v>
       </c>
@@ -5723,33 +5727,33 @@
       </c>
     </row>
     <row r="95" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A95" s="57" t="s">
+      <c r="A95" s="54" t="s">
         <v>1064</v>
       </c>
-      <c r="B95" s="58" t="s">
+      <c r="B95" s="55" t="s">
         <v>1068</v>
       </c>
-      <c r="C95" s="52">
+      <c r="C95" s="60">
         <v>1</v>
       </c>
-      <c r="D95" s="57" t="s">
+      <c r="D95" s="54" t="s">
         <v>279</v>
       </c>
       <c r="E95" s="36">
         <v>447</v>
       </c>
       <c r="F95" s="23" t="s">
-        <v>564</v>
+        <v>1095</v>
       </c>
       <c r="G95" s="23" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="62" customHeight="1">
-      <c r="A96" s="55"/>
-      <c r="B96" s="59"/>
-      <c r="C96" s="53"/>
-      <c r="D96" s="55"/>
+      <c r="A96" s="52"/>
+      <c r="B96" s="56"/>
+      <c r="C96" s="58"/>
+      <c r="D96" s="52"/>
       <c r="E96" s="29">
         <v>105</v>
       </c>
@@ -5761,10 +5765,10 @@
       </c>
     </row>
     <row r="97" spans="1:7" ht="62" customHeight="1">
-      <c r="A97" s="55"/>
-      <c r="B97" s="59"/>
-      <c r="C97" s="53"/>
-      <c r="D97" s="55"/>
+      <c r="A97" s="52"/>
+      <c r="B97" s="56"/>
+      <c r="C97" s="58"/>
+      <c r="D97" s="52"/>
       <c r="E97" s="29">
         <v>314</v>
       </c>
@@ -5776,12 +5780,12 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="62" customHeight="1">
-      <c r="A98" s="55"/>
-      <c r="B98" s="59"/>
-      <c r="C98" s="53">
+      <c r="A98" s="52"/>
+      <c r="B98" s="56"/>
+      <c r="C98" s="58">
         <v>2</v>
       </c>
-      <c r="D98" s="55" t="s">
+      <c r="D98" s="52" t="s">
         <v>257</v>
       </c>
       <c r="E98" s="29">
@@ -5795,10 +5799,10 @@
       </c>
     </row>
     <row r="99" spans="1:7" ht="62" customHeight="1">
-      <c r="A99" s="55"/>
-      <c r="B99" s="59"/>
-      <c r="C99" s="53"/>
-      <c r="D99" s="55"/>
+      <c r="A99" s="52"/>
+      <c r="B99" s="56"/>
+      <c r="C99" s="58"/>
+      <c r="D99" s="52"/>
       <c r="E99" s="29">
         <v>124</v>
       </c>
@@ -5810,10 +5814,10 @@
       </c>
     </row>
     <row r="100" spans="1:7" ht="62" customHeight="1">
-      <c r="A100" s="55"/>
-      <c r="B100" s="59"/>
-      <c r="C100" s="53"/>
-      <c r="D100" s="55"/>
+      <c r="A100" s="52"/>
+      <c r="B100" s="56"/>
+      <c r="C100" s="58"/>
+      <c r="D100" s="52"/>
       <c r="E100" s="29">
         <v>290</v>
       </c>
@@ -5825,12 +5829,12 @@
       </c>
     </row>
     <row r="101" spans="1:7" ht="62" customHeight="1">
-      <c r="A101" s="55"/>
-      <c r="B101" s="59"/>
-      <c r="C101" s="53">
+      <c r="A101" s="52"/>
+      <c r="B101" s="56"/>
+      <c r="C101" s="58">
         <v>3</v>
       </c>
-      <c r="D101" s="55" t="s">
+      <c r="D101" s="52" t="s">
         <v>548</v>
       </c>
       <c r="E101" s="29">
@@ -5844,10 +5848,10 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="62" customHeight="1">
-      <c r="A102" s="55"/>
-      <c r="B102" s="59"/>
-      <c r="C102" s="53"/>
-      <c r="D102" s="55"/>
+      <c r="A102" s="52"/>
+      <c r="B102" s="56"/>
+      <c r="C102" s="58"/>
+      <c r="D102" s="52"/>
       <c r="E102" s="29">
         <v>293</v>
       </c>
@@ -5859,10 +5863,10 @@
       </c>
     </row>
     <row r="103" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A103" s="56"/>
-      <c r="B103" s="60"/>
-      <c r="C103" s="54"/>
-      <c r="D103" s="56"/>
+      <c r="A103" s="53"/>
+      <c r="B103" s="57"/>
+      <c r="C103" s="59"/>
+      <c r="D103" s="53"/>
       <c r="E103" s="37">
         <v>449</v>
       </c>
@@ -5874,16 +5878,16 @@
       </c>
     </row>
     <row r="104" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A104" s="57" t="s">
+      <c r="A104" s="54" t="s">
         <v>1064</v>
       </c>
-      <c r="B104" s="58" t="s">
+      <c r="B104" s="55" t="s">
         <v>1069</v>
       </c>
-      <c r="C104" s="52">
+      <c r="C104" s="60">
         <v>1</v>
       </c>
-      <c r="D104" s="57" t="s">
+      <c r="D104" s="54" t="s">
         <v>181</v>
       </c>
       <c r="E104" s="36">
@@ -5897,10 +5901,10 @@
       </c>
     </row>
     <row r="105" spans="1:7" ht="62" customHeight="1">
-      <c r="A105" s="55"/>
-      <c r="B105" s="59"/>
-      <c r="C105" s="53"/>
-      <c r="D105" s="55"/>
+      <c r="A105" s="52"/>
+      <c r="B105" s="56"/>
+      <c r="C105" s="58"/>
+      <c r="D105" s="52"/>
       <c r="E105" s="29">
         <v>182</v>
       </c>
@@ -5912,10 +5916,10 @@
       </c>
     </row>
     <row r="106" spans="1:7" ht="62" customHeight="1">
-      <c r="A106" s="55"/>
-      <c r="B106" s="59"/>
-      <c r="C106" s="53"/>
-      <c r="D106" s="55"/>
+      <c r="A106" s="52"/>
+      <c r="B106" s="56"/>
+      <c r="C106" s="58"/>
+      <c r="D106" s="52"/>
       <c r="E106" s="29">
         <v>414</v>
       </c>
@@ -5927,10 +5931,10 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="62" customHeight="1">
-      <c r="A107" s="55"/>
-      <c r="B107" s="59"/>
-      <c r="C107" s="53"/>
-      <c r="D107" s="55"/>
+      <c r="A107" s="52"/>
+      <c r="B107" s="56"/>
+      <c r="C107" s="58"/>
+      <c r="D107" s="52"/>
       <c r="E107" s="29">
         <v>445</v>
       </c>
@@ -5942,12 +5946,12 @@
       </c>
     </row>
     <row r="108" spans="1:7" ht="62" customHeight="1">
-      <c r="A108" s="55"/>
-      <c r="B108" s="59"/>
-      <c r="C108" s="53">
+      <c r="A108" s="52"/>
+      <c r="B108" s="56"/>
+      <c r="C108" s="58">
         <v>2</v>
       </c>
-      <c r="D108" s="55" t="s">
+      <c r="D108" s="52" t="s">
         <v>214</v>
       </c>
       <c r="E108" s="29">
@@ -5961,10 +5965,10 @@
       </c>
     </row>
     <row r="109" spans="1:7" ht="62" customHeight="1">
-      <c r="A109" s="55"/>
-      <c r="B109" s="59"/>
-      <c r="C109" s="53"/>
-      <c r="D109" s="55"/>
+      <c r="A109" s="52"/>
+      <c r="B109" s="56"/>
+      <c r="C109" s="58"/>
+      <c r="D109" s="52"/>
       <c r="E109" s="29">
         <v>340</v>
       </c>
@@ -5976,10 +5980,10 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="62" customHeight="1">
-      <c r="A110" s="55"/>
-      <c r="B110" s="59"/>
-      <c r="C110" s="53"/>
-      <c r="D110" s="55"/>
+      <c r="A110" s="52"/>
+      <c r="B110" s="56"/>
+      <c r="C110" s="58"/>
+      <c r="D110" s="52"/>
       <c r="E110" s="29">
         <v>111</v>
       </c>
@@ -5991,10 +5995,10 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="62" customHeight="1">
-      <c r="A111" s="55"/>
-      <c r="B111" s="59"/>
-      <c r="C111" s="53"/>
-      <c r="D111" s="55"/>
+      <c r="A111" s="52"/>
+      <c r="B111" s="56"/>
+      <c r="C111" s="58"/>
+      <c r="D111" s="52"/>
       <c r="E111" s="29">
         <v>371</v>
       </c>
@@ -6006,12 +6010,12 @@
       </c>
     </row>
     <row r="112" spans="1:7" ht="62" customHeight="1">
-      <c r="A112" s="55"/>
-      <c r="B112" s="59"/>
-      <c r="C112" s="53">
+      <c r="A112" s="52"/>
+      <c r="B112" s="56"/>
+      <c r="C112" s="58">
         <v>3</v>
       </c>
-      <c r="D112" s="55" t="s">
+      <c r="D112" s="52" t="s">
         <v>176</v>
       </c>
       <c r="E112" s="29">
@@ -6025,10 +6029,10 @@
       </c>
     </row>
     <row r="113" spans="1:7" ht="62" customHeight="1">
-      <c r="A113" s="55"/>
-      <c r="B113" s="59"/>
-      <c r="C113" s="53"/>
-      <c r="D113" s="55"/>
+      <c r="A113" s="52"/>
+      <c r="B113" s="56"/>
+      <c r="C113" s="58"/>
+      <c r="D113" s="52"/>
       <c r="E113" s="29">
         <v>47</v>
       </c>
@@ -6040,10 +6044,10 @@
       </c>
     </row>
     <row r="114" spans="1:7" ht="62" customHeight="1">
-      <c r="A114" s="55"/>
-      <c r="B114" s="59"/>
-      <c r="C114" s="53"/>
-      <c r="D114" s="55"/>
+      <c r="A114" s="52"/>
+      <c r="B114" s="56"/>
+      <c r="C114" s="58"/>
+      <c r="D114" s="52"/>
       <c r="E114" s="29">
         <v>347</v>
       </c>
@@ -6055,10 +6059,10 @@
       </c>
     </row>
     <row r="115" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A115" s="56"/>
-      <c r="B115" s="60"/>
-      <c r="C115" s="54"/>
-      <c r="D115" s="56"/>
+      <c r="A115" s="53"/>
+      <c r="B115" s="57"/>
+      <c r="C115" s="59"/>
+      <c r="D115" s="53"/>
       <c r="E115" s="37">
         <v>487</v>
       </c>
@@ -6070,16 +6074,16 @@
       </c>
     </row>
     <row r="116" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A116" s="57" t="s">
+      <c r="A116" s="54" t="s">
         <v>1064</v>
       </c>
-      <c r="B116" s="58" t="s">
+      <c r="B116" s="55" t="s">
         <v>1070</v>
       </c>
-      <c r="C116" s="52">
+      <c r="C116" s="60">
         <v>1</v>
       </c>
-      <c r="D116" s="57" t="s">
+      <c r="D116" s="54" t="s">
         <v>278</v>
       </c>
       <c r="E116" s="36">
@@ -6093,10 +6097,10 @@
       </c>
     </row>
     <row r="117" spans="1:7" ht="62" customHeight="1">
-      <c r="A117" s="55"/>
-      <c r="B117" s="59"/>
-      <c r="C117" s="53"/>
-      <c r="D117" s="55"/>
+      <c r="A117" s="52"/>
+      <c r="B117" s="56"/>
+      <c r="C117" s="58"/>
+      <c r="D117" s="52"/>
       <c r="E117" s="29">
         <v>97</v>
       </c>
@@ -6108,10 +6112,10 @@
       </c>
     </row>
     <row r="118" spans="1:7" ht="62" customHeight="1">
-      <c r="A118" s="55"/>
-      <c r="B118" s="59"/>
-      <c r="C118" s="53"/>
-      <c r="D118" s="55"/>
+      <c r="A118" s="52"/>
+      <c r="B118" s="56"/>
+      <c r="C118" s="58"/>
+      <c r="D118" s="52"/>
       <c r="E118" s="29">
         <v>152</v>
       </c>
@@ -6123,10 +6127,10 @@
       </c>
     </row>
     <row r="119" spans="1:7" ht="62" customHeight="1">
-      <c r="A119" s="55"/>
-      <c r="B119" s="59"/>
-      <c r="C119" s="53"/>
-      <c r="D119" s="55"/>
+      <c r="A119" s="52"/>
+      <c r="B119" s="56"/>
+      <c r="C119" s="58"/>
+      <c r="D119" s="52"/>
       <c r="E119" s="29">
         <v>317</v>
       </c>
@@ -6138,12 +6142,12 @@
       </c>
     </row>
     <row r="120" spans="1:7" ht="62" customHeight="1">
-      <c r="A120" s="55"/>
-      <c r="B120" s="59"/>
-      <c r="C120" s="53">
+      <c r="A120" s="52"/>
+      <c r="B120" s="56"/>
+      <c r="C120" s="58">
         <v>2</v>
       </c>
-      <c r="D120" s="55" t="s">
+      <c r="D120" s="52" t="s">
         <v>282</v>
       </c>
       <c r="E120" s="29">
@@ -6157,10 +6161,10 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="62" customHeight="1">
-      <c r="A121" s="55"/>
-      <c r="B121" s="59"/>
-      <c r="C121" s="53"/>
-      <c r="D121" s="55"/>
+      <c r="A121" s="52"/>
+      <c r="B121" s="56"/>
+      <c r="C121" s="58"/>
+      <c r="D121" s="52"/>
       <c r="E121" s="29">
         <v>301</v>
       </c>
@@ -6172,10 +6176,10 @@
       </c>
     </row>
     <row r="122" spans="1:7" ht="62" customHeight="1">
-      <c r="A122" s="55"/>
-      <c r="B122" s="59"/>
-      <c r="C122" s="53"/>
-      <c r="D122" s="55"/>
+      <c r="A122" s="52"/>
+      <c r="B122" s="56"/>
+      <c r="C122" s="58"/>
+      <c r="D122" s="52"/>
       <c r="E122" s="29">
         <v>334</v>
       </c>
@@ -6187,10 +6191,10 @@
       </c>
     </row>
     <row r="123" spans="1:7" ht="62" customHeight="1">
-      <c r="A123" s="55"/>
-      <c r="B123" s="59"/>
-      <c r="C123" s="53"/>
-      <c r="D123" s="55"/>
+      <c r="A123" s="52"/>
+      <c r="B123" s="56"/>
+      <c r="C123" s="58"/>
+      <c r="D123" s="52"/>
       <c r="E123" s="29">
         <v>421</v>
       </c>
@@ -6202,12 +6206,12 @@
       </c>
     </row>
     <row r="124" spans="1:7" ht="62" customHeight="1">
-      <c r="A124" s="55"/>
-      <c r="B124" s="59"/>
-      <c r="C124" s="53">
+      <c r="A124" s="52"/>
+      <c r="B124" s="56"/>
+      <c r="C124" s="58">
         <v>3</v>
       </c>
-      <c r="D124" s="55" t="s">
+      <c r="D124" s="52" t="s">
         <v>150</v>
       </c>
       <c r="E124" s="29">
@@ -6221,10 +6225,10 @@
       </c>
     </row>
     <row r="125" spans="1:7" ht="62" customHeight="1">
-      <c r="A125" s="55"/>
-      <c r="B125" s="59"/>
-      <c r="C125" s="53"/>
-      <c r="D125" s="55"/>
+      <c r="A125" s="52"/>
+      <c r="B125" s="56"/>
+      <c r="C125" s="58"/>
+      <c r="D125" s="52"/>
       <c r="E125" s="29">
         <v>61</v>
       </c>
@@ -6236,10 +6240,10 @@
       </c>
     </row>
     <row r="126" spans="1:7" ht="62" customHeight="1">
-      <c r="A126" s="55"/>
-      <c r="B126" s="59"/>
-      <c r="C126" s="53"/>
-      <c r="D126" s="55"/>
+      <c r="A126" s="52"/>
+      <c r="B126" s="56"/>
+      <c r="C126" s="58"/>
+      <c r="D126" s="52"/>
       <c r="E126" s="29">
         <v>24</v>
       </c>
@@ -6251,10 +6255,10 @@
       </c>
     </row>
     <row r="127" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A127" s="56"/>
-      <c r="B127" s="60"/>
-      <c r="C127" s="54"/>
-      <c r="D127" s="56"/>
+      <c r="A127" s="53"/>
+      <c r="B127" s="57"/>
+      <c r="C127" s="59"/>
+      <c r="D127" s="53"/>
       <c r="E127" s="37">
         <v>132</v>
       </c>
@@ -6266,16 +6270,16 @@
       </c>
     </row>
     <row r="128" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A128" s="57" t="s">
+      <c r="A128" s="54" t="s">
         <v>1065</v>
       </c>
-      <c r="B128" s="58" t="s">
+      <c r="B128" s="55" t="s">
         <v>1067</v>
       </c>
-      <c r="C128" s="52">
+      <c r="C128" s="60">
         <v>1</v>
       </c>
-      <c r="D128" s="57" t="s">
+      <c r="D128" s="54" t="s">
         <v>495</v>
       </c>
       <c r="E128" s="36">
@@ -6289,10 +6293,10 @@
       </c>
     </row>
     <row r="129" spans="1:7" ht="62" customHeight="1">
-      <c r="A129" s="55"/>
-      <c r="B129" s="59"/>
-      <c r="C129" s="53"/>
-      <c r="D129" s="55"/>
+      <c r="A129" s="52"/>
+      <c r="B129" s="56"/>
+      <c r="C129" s="58"/>
+      <c r="D129" s="52"/>
       <c r="E129" s="29">
         <v>405</v>
       </c>
@@ -6304,10 +6308,10 @@
       </c>
     </row>
     <row r="130" spans="1:7" ht="62" customHeight="1">
-      <c r="A130" s="55"/>
-      <c r="B130" s="59"/>
-      <c r="C130" s="53"/>
-      <c r="D130" s="55"/>
+      <c r="A130" s="52"/>
+      <c r="B130" s="56"/>
+      <c r="C130" s="58"/>
+      <c r="D130" s="52"/>
       <c r="E130" s="29">
         <v>483</v>
       </c>
@@ -6319,12 +6323,12 @@
       </c>
     </row>
     <row r="131" spans="1:7" ht="62" customHeight="1">
-      <c r="A131" s="55"/>
-      <c r="B131" s="59"/>
-      <c r="C131" s="53">
+      <c r="A131" s="52"/>
+      <c r="B131" s="56"/>
+      <c r="C131" s="58">
         <v>2</v>
       </c>
-      <c r="D131" s="55" t="s">
+      <c r="D131" s="52" t="s">
         <v>283</v>
       </c>
       <c r="E131" s="29">
@@ -6338,10 +6342,10 @@
       </c>
     </row>
     <row r="132" spans="1:7" ht="62" customHeight="1">
-      <c r="A132" s="55"/>
-      <c r="B132" s="59"/>
-      <c r="C132" s="53"/>
-      <c r="D132" s="55"/>
+      <c r="A132" s="52"/>
+      <c r="B132" s="56"/>
+      <c r="C132" s="58"/>
+      <c r="D132" s="52"/>
       <c r="E132" s="29">
         <v>151</v>
       </c>
@@ -6353,12 +6357,12 @@
       </c>
     </row>
     <row r="133" spans="1:7" ht="62" customHeight="1">
-      <c r="A133" s="55"/>
-      <c r="B133" s="59"/>
-      <c r="C133" s="53">
+      <c r="A133" s="52"/>
+      <c r="B133" s="56"/>
+      <c r="C133" s="58">
         <v>3</v>
       </c>
-      <c r="D133" s="55" t="s">
+      <c r="D133" s="52" t="s">
         <v>276</v>
       </c>
       <c r="E133" s="29">
@@ -6372,10 +6376,10 @@
       </c>
     </row>
     <row r="134" spans="1:7" ht="62" customHeight="1">
-      <c r="A134" s="55"/>
-      <c r="B134" s="59"/>
-      <c r="C134" s="53"/>
-      <c r="D134" s="55"/>
+      <c r="A134" s="52"/>
+      <c r="B134" s="56"/>
+      <c r="C134" s="58"/>
+      <c r="D134" s="52"/>
       <c r="E134" s="29">
         <v>493</v>
       </c>
@@ -6387,10 +6391,10 @@
       </c>
     </row>
     <row r="135" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A135" s="56"/>
-      <c r="B135" s="60"/>
-      <c r="C135" s="54"/>
-      <c r="D135" s="56"/>
+      <c r="A135" s="53"/>
+      <c r="B135" s="57"/>
+      <c r="C135" s="59"/>
+      <c r="D135" s="53"/>
       <c r="E135" s="37">
         <v>256</v>
       </c>
@@ -6402,16 +6406,16 @@
       </c>
     </row>
     <row r="136" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A136" s="57" t="s">
+      <c r="A136" s="54" t="s">
         <v>1065</v>
       </c>
-      <c r="B136" s="58" t="s">
+      <c r="B136" s="55" t="s">
         <v>1068</v>
       </c>
-      <c r="C136" s="52">
+      <c r="C136" s="60">
         <v>1</v>
       </c>
-      <c r="D136" s="57" t="s">
+      <c r="D136" s="54" t="s">
         <v>224</v>
       </c>
       <c r="E136" s="36">
@@ -6425,10 +6429,10 @@
       </c>
     </row>
     <row r="137" spans="1:7" ht="62" customHeight="1">
-      <c r="A137" s="55"/>
-      <c r="B137" s="59"/>
-      <c r="C137" s="53"/>
-      <c r="D137" s="55"/>
+      <c r="A137" s="52"/>
+      <c r="B137" s="56"/>
+      <c r="C137" s="58"/>
+      <c r="D137" s="52"/>
       <c r="E137" s="29">
         <v>374</v>
       </c>
@@ -6440,10 +6444,10 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="62" customHeight="1">
-      <c r="A138" s="55"/>
-      <c r="B138" s="59"/>
-      <c r="C138" s="53"/>
-      <c r="D138" s="55"/>
+      <c r="A138" s="52"/>
+      <c r="B138" s="56"/>
+      <c r="C138" s="58"/>
+      <c r="D138" s="52"/>
       <c r="E138" s="29">
         <v>195</v>
       </c>
@@ -6455,12 +6459,12 @@
       </c>
     </row>
     <row r="139" spans="1:7" ht="62" customHeight="1">
-      <c r="A139" s="55"/>
-      <c r="B139" s="59"/>
-      <c r="C139" s="53">
+      <c r="A139" s="52"/>
+      <c r="B139" s="56"/>
+      <c r="C139" s="58">
         <v>2</v>
       </c>
-      <c r="D139" s="55" t="s">
+      <c r="D139" s="52" t="s">
         <v>280</v>
       </c>
       <c r="E139" s="29">
@@ -6474,10 +6478,10 @@
       </c>
     </row>
     <row r="140" spans="1:7" ht="62" customHeight="1">
-      <c r="A140" s="55"/>
-      <c r="B140" s="59"/>
-      <c r="C140" s="53"/>
-      <c r="D140" s="55"/>
+      <c r="A140" s="52"/>
+      <c r="B140" s="56"/>
+      <c r="C140" s="58"/>
+      <c r="D140" s="52"/>
       <c r="E140" s="29">
         <v>270</v>
       </c>
@@ -6489,10 +6493,10 @@
       </c>
     </row>
     <row r="141" spans="1:7" ht="62" customHeight="1">
-      <c r="A141" s="55"/>
-      <c r="B141" s="59"/>
-      <c r="C141" s="53"/>
-      <c r="D141" s="55"/>
+      <c r="A141" s="52"/>
+      <c r="B141" s="56"/>
+      <c r="C141" s="58"/>
+      <c r="D141" s="52"/>
       <c r="E141" s="29">
         <v>471</v>
       </c>
@@ -6504,12 +6508,12 @@
       </c>
     </row>
     <row r="142" spans="1:7" ht="62" customHeight="1">
-      <c r="A142" s="55"/>
-      <c r="B142" s="59"/>
-      <c r="C142" s="53">
+      <c r="A142" s="52"/>
+      <c r="B142" s="56"/>
+      <c r="C142" s="58">
         <v>3</v>
       </c>
-      <c r="D142" s="55" t="s">
+      <c r="D142" s="52" t="s">
         <v>203</v>
       </c>
       <c r="E142" s="29">
@@ -6523,10 +6527,10 @@
       </c>
     </row>
     <row r="143" spans="1:7" ht="62" customHeight="1">
-      <c r="A143" s="55"/>
-      <c r="B143" s="59"/>
-      <c r="C143" s="53"/>
-      <c r="D143" s="55"/>
+      <c r="A143" s="52"/>
+      <c r="B143" s="56"/>
+      <c r="C143" s="58"/>
+      <c r="D143" s="52"/>
       <c r="E143" s="29">
         <v>76</v>
       </c>
@@ -6538,10 +6542,10 @@
       </c>
     </row>
     <row r="144" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A144" s="56"/>
-      <c r="B144" s="60"/>
-      <c r="C144" s="54"/>
-      <c r="D144" s="56"/>
+      <c r="A144" s="53"/>
+      <c r="B144" s="57"/>
+      <c r="C144" s="59"/>
+      <c r="D144" s="53"/>
       <c r="E144" s="37">
         <v>207</v>
       </c>
@@ -6553,16 +6557,16 @@
       </c>
     </row>
     <row r="145" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A145" s="57" t="s">
+      <c r="A145" s="54" t="s">
         <v>1065</v>
       </c>
-      <c r="B145" s="58" t="s">
+      <c r="B145" s="55" t="s">
         <v>1071</v>
       </c>
-      <c r="C145" s="52">
+      <c r="C145" s="60">
         <v>1</v>
       </c>
-      <c r="D145" s="57" t="s">
+      <c r="D145" s="54" t="s">
         <v>281</v>
       </c>
       <c r="E145" s="36">
@@ -6576,10 +6580,10 @@
       </c>
     </row>
     <row r="146" spans="1:7" ht="62" customHeight="1">
-      <c r="A146" s="55"/>
-      <c r="B146" s="59"/>
-      <c r="C146" s="53"/>
-      <c r="D146" s="55"/>
+      <c r="A146" s="52"/>
+      <c r="B146" s="56"/>
+      <c r="C146" s="58"/>
+      <c r="D146" s="52"/>
       <c r="E146" s="29">
         <v>406</v>
       </c>
@@ -6591,10 +6595,10 @@
       </c>
     </row>
     <row r="147" spans="1:7" ht="62" customHeight="1">
-      <c r="A147" s="55"/>
-      <c r="B147" s="59"/>
-      <c r="C147" s="53"/>
-      <c r="D147" s="55"/>
+      <c r="A147" s="52"/>
+      <c r="B147" s="56"/>
+      <c r="C147" s="58"/>
+      <c r="D147" s="52"/>
       <c r="E147" s="29">
         <v>279</v>
       </c>
@@ -6606,12 +6610,12 @@
       </c>
     </row>
     <row r="148" spans="1:7" ht="62" customHeight="1">
-      <c r="A148" s="55"/>
-      <c r="B148" s="59"/>
-      <c r="C148" s="53">
+      <c r="A148" s="52"/>
+      <c r="B148" s="56"/>
+      <c r="C148" s="58">
         <v>2</v>
       </c>
-      <c r="D148" s="55" t="s">
+      <c r="D148" s="52" t="s">
         <v>277</v>
       </c>
       <c r="E148" s="29">
@@ -6625,10 +6629,10 @@
       </c>
     </row>
     <row r="149" spans="1:7" ht="62" customHeight="1">
-      <c r="A149" s="55"/>
-      <c r="B149" s="59"/>
-      <c r="C149" s="53"/>
-      <c r="D149" s="55"/>
+      <c r="A149" s="52"/>
+      <c r="B149" s="56"/>
+      <c r="C149" s="58"/>
+      <c r="D149" s="52"/>
       <c r="E149" s="29">
         <v>69</v>
       </c>
@@ -6640,10 +6644,10 @@
       </c>
     </row>
     <row r="150" spans="1:7" ht="62" customHeight="1">
-      <c r="A150" s="55"/>
-      <c r="B150" s="59"/>
-      <c r="C150" s="53"/>
-      <c r="D150" s="55"/>
+      <c r="A150" s="52"/>
+      <c r="B150" s="56"/>
+      <c r="C150" s="58"/>
+      <c r="D150" s="52"/>
       <c r="E150" s="29">
         <v>378</v>
       </c>
@@ -6655,12 +6659,12 @@
       </c>
     </row>
     <row r="151" spans="1:7" ht="62" customHeight="1">
-      <c r="A151" s="55"/>
-      <c r="B151" s="59"/>
-      <c r="C151" s="53">
+      <c r="A151" s="52"/>
+      <c r="B151" s="56"/>
+      <c r="C151" s="58">
         <v>3</v>
       </c>
-      <c r="D151" s="55" t="s">
+      <c r="D151" s="52" t="s">
         <v>448</v>
       </c>
       <c r="E151" s="29">
@@ -6674,10 +6678,10 @@
       </c>
     </row>
     <row r="152" spans="1:7" ht="62" customHeight="1">
-      <c r="A152" s="55"/>
-      <c r="B152" s="59"/>
-      <c r="C152" s="53"/>
-      <c r="D152" s="55"/>
+      <c r="A152" s="52"/>
+      <c r="B152" s="56"/>
+      <c r="C152" s="58"/>
+      <c r="D152" s="52"/>
       <c r="E152" s="29">
         <v>167</v>
       </c>
@@ -6689,10 +6693,10 @@
       </c>
     </row>
     <row r="153" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A153" s="56"/>
-      <c r="B153" s="60"/>
-      <c r="C153" s="54"/>
-      <c r="D153" s="56"/>
+      <c r="A153" s="53"/>
+      <c r="B153" s="57"/>
+      <c r="C153" s="59"/>
+      <c r="D153" s="53"/>
       <c r="E153" s="37">
         <v>326</v>
       </c>
@@ -6704,16 +6708,16 @@
       </c>
     </row>
     <row r="154" spans="1:7" s="16" customFormat="1" ht="62" customHeight="1">
-      <c r="A154" s="57" t="s">
+      <c r="A154" s="54" t="s">
         <v>1065</v>
       </c>
-      <c r="B154" s="58" t="s">
+      <c r="B154" s="55" t="s">
         <v>1072</v>
       </c>
-      <c r="C154" s="52">
+      <c r="C154" s="60">
         <v>1</v>
       </c>
-      <c r="D154" s="57" t="s">
+      <c r="D154" s="54" t="s">
         <v>442</v>
       </c>
       <c r="E154" s="36">
@@ -6727,10 +6731,10 @@
       </c>
     </row>
     <row r="155" spans="1:7" ht="62" customHeight="1">
-      <c r="A155" s="55"/>
-      <c r="B155" s="59"/>
-      <c r="C155" s="53"/>
-      <c r="D155" s="55"/>
+      <c r="A155" s="52"/>
+      <c r="B155" s="56"/>
+      <c r="C155" s="58"/>
+      <c r="D155" s="52"/>
       <c r="E155" s="29">
         <v>203</v>
       </c>
@@ -6742,10 +6746,10 @@
       </c>
     </row>
     <row r="156" spans="1:7" ht="62" customHeight="1">
-      <c r="A156" s="55"/>
-      <c r="B156" s="59"/>
-      <c r="C156" s="53"/>
-      <c r="D156" s="55"/>
+      <c r="A156" s="52"/>
+      <c r="B156" s="56"/>
+      <c r="C156" s="58"/>
+      <c r="D156" s="52"/>
       <c r="E156" s="29">
         <v>398</v>
       </c>
@@ -6757,12 +6761,12 @@
       </c>
     </row>
     <row r="157" spans="1:7" ht="62" customHeight="1">
-      <c r="A157" s="55"/>
-      <c r="B157" s="59"/>
-      <c r="C157" s="53">
+      <c r="A157" s="52"/>
+      <c r="B157" s="56"/>
+      <c r="C157" s="58">
         <v>2</v>
       </c>
-      <c r="D157" s="55" t="s">
+      <c r="D157" s="52" t="s">
         <v>284</v>
       </c>
       <c r="E157" s="29">
@@ -6776,10 +6780,10 @@
       </c>
     </row>
     <row r="158" spans="1:7" ht="62" customHeight="1">
-      <c r="A158" s="55"/>
-      <c r="B158" s="59"/>
-      <c r="C158" s="53"/>
-      <c r="D158" s="55"/>
+      <c r="A158" s="52"/>
+      <c r="B158" s="56"/>
+      <c r="C158" s="58"/>
+      <c r="D158" s="52"/>
       <c r="E158" s="29">
         <v>53</v>
       </c>
@@ -6791,10 +6795,10 @@
       </c>
     </row>
     <row r="159" spans="1:7" ht="62" customHeight="1">
-      <c r="A159" s="55"/>
-      <c r="B159" s="59"/>
-      <c r="C159" s="53"/>
-      <c r="D159" s="55"/>
+      <c r="A159" s="52"/>
+      <c r="B159" s="56"/>
+      <c r="C159" s="58"/>
+      <c r="D159" s="52"/>
       <c r="E159" s="29">
         <v>320</v>
       </c>
@@ -6806,12 +6810,12 @@
       </c>
     </row>
     <row r="160" spans="1:7" ht="62" customHeight="1">
-      <c r="A160" s="55"/>
-      <c r="B160" s="59"/>
-      <c r="C160" s="53">
+      <c r="A160" s="52"/>
+      <c r="B160" s="56"/>
+      <c r="C160" s="58">
         <v>3</v>
       </c>
-      <c r="D160" s="55" t="s">
+      <c r="D160" s="52" t="s">
         <v>285</v>
       </c>
       <c r="E160" s="29">
@@ -6825,10 +6829,10 @@
       </c>
     </row>
     <row r="161" spans="1:7" ht="62" customHeight="1">
-      <c r="A161" s="55"/>
-      <c r="B161" s="59"/>
-      <c r="C161" s="53"/>
-      <c r="D161" s="55"/>
+      <c r="A161" s="52"/>
+      <c r="B161" s="56"/>
+      <c r="C161" s="58"/>
+      <c r="D161" s="52"/>
       <c r="E161" s="29">
         <v>85</v>
       </c>
@@ -6840,10 +6844,10 @@
       </c>
     </row>
     <row r="162" spans="1:7" s="14" customFormat="1" ht="62" customHeight="1" thickBot="1">
-      <c r="A162" s="56"/>
-      <c r="B162" s="60"/>
-      <c r="C162" s="54"/>
-      <c r="D162" s="56"/>
+      <c r="A162" s="53"/>
+      <c r="B162" s="57"/>
+      <c r="C162" s="59"/>
+      <c r="D162" s="53"/>
       <c r="E162" s="37">
         <v>121</v>
       </c>
@@ -6862,18 +6866,86 @@
     </row>
   </sheetData>
   <mergeCells count="128">
-    <mergeCell ref="D124:D127"/>
-    <mergeCell ref="D128:D130"/>
-    <mergeCell ref="A128:A135"/>
-    <mergeCell ref="B128:B135"/>
-    <mergeCell ref="C131:C132"/>
-    <mergeCell ref="D131:D132"/>
-    <mergeCell ref="A154:A162"/>
-    <mergeCell ref="A136:A144"/>
-    <mergeCell ref="A145:A153"/>
-    <mergeCell ref="B145:B153"/>
-    <mergeCell ref="B154:B162"/>
-    <mergeCell ref="B136:B144"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="C82:C85"/>
+    <mergeCell ref="C78:C81"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D145:D147"/>
+    <mergeCell ref="D148:D150"/>
+    <mergeCell ref="D151:D153"/>
+    <mergeCell ref="D154:D156"/>
+    <mergeCell ref="D157:D159"/>
+    <mergeCell ref="D133:D135"/>
+    <mergeCell ref="D136:D138"/>
+    <mergeCell ref="D139:D141"/>
+    <mergeCell ref="C104:C107"/>
+    <mergeCell ref="C128:C130"/>
+    <mergeCell ref="C124:C127"/>
+    <mergeCell ref="C120:C123"/>
+    <mergeCell ref="C116:C119"/>
+    <mergeCell ref="C112:C115"/>
+    <mergeCell ref="C108:C111"/>
+    <mergeCell ref="D101:D103"/>
+    <mergeCell ref="D104:D107"/>
+    <mergeCell ref="D108:D111"/>
+    <mergeCell ref="D112:D115"/>
+    <mergeCell ref="D116:D119"/>
+    <mergeCell ref="D120:D123"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D95:D97"/>
+    <mergeCell ref="D98:D100"/>
+    <mergeCell ref="C101:C103"/>
+    <mergeCell ref="C98:C100"/>
+    <mergeCell ref="C95:C97"/>
+    <mergeCell ref="C92:C94"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="D82:D85"/>
+    <mergeCell ref="D86:D88"/>
+    <mergeCell ref="D89:D91"/>
+    <mergeCell ref="D92:D94"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="D59:D61"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="D70:D73"/>
+    <mergeCell ref="D74:D77"/>
+    <mergeCell ref="D78:D81"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="D36:D39"/>
     <mergeCell ref="B2:B10"/>
     <mergeCell ref="B11:B19"/>
     <mergeCell ref="B20:B31"/>
@@ -6898,45 +6970,18 @@
     <mergeCell ref="A44:A52"/>
     <mergeCell ref="B44:B52"/>
     <mergeCell ref="B86:B94"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="D82:D85"/>
-    <mergeCell ref="D86:D88"/>
-    <mergeCell ref="D89:D91"/>
-    <mergeCell ref="D92:D94"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="D59:D61"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="D74:D77"/>
-    <mergeCell ref="D78:D81"/>
-    <mergeCell ref="D101:D103"/>
-    <mergeCell ref="D104:D107"/>
-    <mergeCell ref="D108:D111"/>
-    <mergeCell ref="D112:D115"/>
-    <mergeCell ref="D116:D119"/>
-    <mergeCell ref="D120:D123"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D95:D97"/>
-    <mergeCell ref="D98:D100"/>
+    <mergeCell ref="D124:D127"/>
+    <mergeCell ref="D128:D130"/>
+    <mergeCell ref="A128:A135"/>
+    <mergeCell ref="B128:B135"/>
+    <mergeCell ref="C131:C132"/>
+    <mergeCell ref="D131:D132"/>
+    <mergeCell ref="A154:A162"/>
+    <mergeCell ref="A136:A144"/>
+    <mergeCell ref="A145:A153"/>
+    <mergeCell ref="B145:B153"/>
+    <mergeCell ref="B154:B162"/>
+    <mergeCell ref="B136:B144"/>
     <mergeCell ref="C145:C147"/>
     <mergeCell ref="C142:C144"/>
     <mergeCell ref="C139:C141"/>
@@ -6949,47 +6994,6 @@
     <mergeCell ref="C151:C153"/>
     <mergeCell ref="C148:C150"/>
     <mergeCell ref="D142:D144"/>
-    <mergeCell ref="D145:D147"/>
-    <mergeCell ref="D148:D150"/>
-    <mergeCell ref="D151:D153"/>
-    <mergeCell ref="D154:D156"/>
-    <mergeCell ref="D157:D159"/>
-    <mergeCell ref="D133:D135"/>
-    <mergeCell ref="D136:D138"/>
-    <mergeCell ref="D139:D141"/>
-    <mergeCell ref="C104:C107"/>
-    <mergeCell ref="C101:C103"/>
-    <mergeCell ref="C98:C100"/>
-    <mergeCell ref="C95:C97"/>
-    <mergeCell ref="C92:C94"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="C128:C130"/>
-    <mergeCell ref="C124:C127"/>
-    <mergeCell ref="C120:C123"/>
-    <mergeCell ref="C116:C119"/>
-    <mergeCell ref="C112:C115"/>
-    <mergeCell ref="C108:C111"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="C86:C88"/>
-    <mergeCell ref="C82:C85"/>
-    <mergeCell ref="C78:C81"/>
-    <mergeCell ref="C74:C77"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="C24:C27"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions gridLines="1"/>
@@ -7019,7 +7023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212612BB-E84A-4441-9066-EF49AFBE483D}">
   <dimension ref="A1:BB165"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+    <sheetView zoomScale="99" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>